<commit_message>
Fixed drop columns in init_data.py
* fixed issues in init_data v0.5.0 where 'adult_literacy_pct', 'homicides_per_100k', 'tax_revenue_pct_gdp' not dropped
</commit_message>
<xml_diff>
--- a/output/clean_data_central_africa.xlsx
+++ b/output/clean_data_central_africa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>country_index</t>
   </si>
@@ -55,6 +55,9 @@
     <t>pct_agriculture_employment</t>
   </si>
   <si>
+    <t>gni_index</t>
+  </si>
+  <si>
     <t>pct_industry_employment</t>
   </si>
   <si>
@@ -67,9 +70,6 @@
     <t>fdi_pct_gdp</t>
   </si>
   <si>
-    <t>gni_index</t>
-  </si>
-  <si>
     <t>gdp_usd</t>
   </si>
   <si>
@@ -82,12 +82,6 @@
     <t>internet_usage_pct</t>
   </si>
   <si>
-    <t>homicides_per_100k</t>
-  </si>
-  <si>
-    <t>adult_literacy_pct</t>
-  </si>
-  <si>
     <t>child_mortality_per_1k</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>women_in_parliament</t>
   </si>
   <si>
-    <t>tax_revenue_pct_gdp</t>
-  </si>
-  <si>
     <t>unemployment_pct</t>
   </si>
   <si>
@@ -109,19 +100,82 @@
     <t>urban_population_growth_pct</t>
   </si>
   <si>
+    <t>m_income_group</t>
+  </si>
+  <si>
+    <t>m_access_to_electricity_pop</t>
+  </si>
+  <si>
+    <t>m_access_to_electricity_rural</t>
+  </si>
+  <si>
+    <t>m_access_to_electricity_urban</t>
+  </si>
+  <si>
+    <t>m_CO2_emissions_per_capita</t>
+  </si>
+  <si>
     <t>m_compulsory_edu_yrs</t>
   </si>
   <si>
+    <t>m_pct_female_employment</t>
+  </si>
+  <si>
+    <t>m_pct_male_employment</t>
+  </si>
+  <si>
+    <t>m_pct_agriculture_employment</t>
+  </si>
+  <si>
+    <t>m_pct_industry_employment</t>
+  </si>
+  <si>
+    <t>m_pct_services_employment</t>
+  </si>
+  <si>
+    <t>m_exports_pct_gdp</t>
+  </si>
+  <si>
+    <t>m_fdi_pct_gdp</t>
+  </si>
+  <si>
+    <t>m_gdp_usd</t>
+  </si>
+  <si>
+    <t>m_gdp_growth_pct</t>
+  </si>
+  <si>
     <t>m_incidence_hiv</t>
   </si>
   <si>
+    <t>m_internet_usage_pct</t>
+  </si>
+  <si>
     <t>m_homicides_per_100k</t>
   </si>
   <si>
     <t>m_adult_literacy_pct</t>
   </si>
   <si>
+    <t>m_child_mortality_per_1k</t>
+  </si>
+  <si>
+    <t>m_avg_air_pollution</t>
+  </si>
+  <si>
+    <t>m_women_in_parliament</t>
+  </si>
+  <si>
     <t>m_tax_revenue_pct_gdp</t>
+  </si>
+  <si>
+    <t>m_unemployment_pct</t>
+  </si>
+  <si>
+    <t>m_urban_population_pct</t>
+  </si>
+  <si>
+    <t>m_urban_population_growth_pct</t>
   </si>
   <si>
     <t>Central Africa 1</t>
@@ -575,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:BC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:55">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,8 +744,62 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:55">
       <c r="A2" s="1">
         <v>32</v>
       </c>
@@ -699,16 +807,16 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -735,19 +843,19 @@
         <v>91.10299683</v>
       </c>
       <c r="O2">
+        <v>290</v>
+      </c>
+      <c r="P2">
         <v>2.549000025</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>6.34800005</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>7.76818252</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>2.642421428</v>
-      </c>
-      <c r="S2">
-        <v>290</v>
       </c>
       <c r="T2">
         <v>3093647227</v>
@@ -762,49 +870,103 @@
         <v>1.38</v>
       </c>
       <c r="X2">
-        <v>4</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="Y2">
-        <v>61.56972885</v>
+        <v>47.08506861</v>
       </c>
       <c r="Z2">
-        <v>77.90000000000001</v>
+        <v>30.5</v>
       </c>
       <c r="AA2">
-        <v>47.08506861</v>
+        <v>1.570000052</v>
       </c>
       <c r="AB2">
-        <v>30.5</v>
+        <v>11.761</v>
       </c>
       <c r="AC2">
-        <v>16.92218544</v>
+        <v>5.480228006</v>
       </c>
       <c r="AD2">
-        <v>1.570000052</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>11.761</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>5.480228006</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2">
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
         <v>0</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:55">
       <c r="A3" s="1">
         <v>33</v>
       </c>
@@ -812,16 +974,16 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G3">
         <v>87.87672424</v>
@@ -848,19 +1010,19 @@
         <v>68.65499878</v>
       </c>
       <c r="O3">
+        <v>3310</v>
+      </c>
+      <c r="P3">
         <v>6.922999859</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>24.42200089</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>40.36113967</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>9.718943229000001</v>
-      </c>
-      <c r="S3">
-        <v>3310</v>
       </c>
       <c r="T3">
         <v>1858121723</v>
@@ -875,49 +1037,103 @@
         <v>40.26</v>
       </c>
       <c r="X3">
-        <v>12.6</v>
+        <v>23</v>
       </c>
       <c r="Y3">
-        <v>91.8724823</v>
+        <v>42.09588617</v>
       </c>
       <c r="Z3">
-        <v>23</v>
+        <v>20.8</v>
       </c>
       <c r="AA3">
-        <v>42.09588617</v>
+        <v>10.34799957</v>
       </c>
       <c r="AB3">
-        <v>20.8</v>
+        <v>64.84</v>
       </c>
       <c r="AC3">
-        <v>16.92218544</v>
+        <v>2.315808738</v>
       </c>
       <c r="AD3">
-        <v>10.34799957</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>64.84</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>2.315808738</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
         <v>0</v>
       </c>
       <c r="AJ3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>1</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:55">
       <c r="A4" s="1">
         <v>44</v>
       </c>
@@ -925,16 +1141,16 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G4">
         <v>72.91772460999999</v>
@@ -961,19 +1177,19 @@
         <v>54.98300171</v>
       </c>
       <c r="O4">
+        <v>830</v>
+      </c>
+      <c r="P4">
         <v>15.57699966</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>29.44099998</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>16.87471351</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.72227588</v>
-      </c>
-      <c r="S4">
-        <v>830</v>
       </c>
       <c r="T4">
         <v>647720707.1</v>
@@ -988,31 +1204,31 @@
         <v>6.98</v>
       </c>
       <c r="X4">
-        <v>2.55</v>
+        <v>78.3</v>
       </c>
       <c r="Y4">
-        <v>91.8724823</v>
+        <v>17.11820358</v>
       </c>
       <c r="Z4">
-        <v>78.3</v>
+        <v>3</v>
       </c>
       <c r="AA4">
-        <v>17.11820358</v>
+        <v>4.361999989</v>
       </c>
       <c r="AB4">
-        <v>3</v>
+        <v>28.193</v>
       </c>
       <c r="AC4">
-        <v>16.92218544</v>
+        <v>2.699437729</v>
       </c>
       <c r="AD4">
-        <v>4.361999989</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>28.193</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <v>2.699437729</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1021,16 +1237,70 @@
         <v>0</v>
       </c>
       <c r="AI4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>1</v>
+      </c>
+      <c r="AV4">
+        <v>1</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:55">
       <c r="A5" s="1">
         <v>45</v>
       </c>
@@ -1038,16 +1308,16 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G5">
         <v>13.5</v>
@@ -1074,19 +1344,19 @@
         <v>81.34899901999999</v>
       </c>
       <c r="O5">
+        <v>440</v>
+      </c>
+      <c r="P5">
         <v>12.20400047</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>6.447000027</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>36.83218885</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>5.131664248</v>
-      </c>
-      <c r="S5">
-        <v>440</v>
       </c>
       <c r="T5">
         <v>35917650630</v>
@@ -1101,31 +1371,31 @@
         <v>3</v>
       </c>
       <c r="X5">
-        <v>2.55</v>
+        <v>101</v>
       </c>
       <c r="Y5">
-        <v>91.8724823</v>
+        <v>46.57451961</v>
       </c>
       <c r="Z5">
-        <v>101</v>
+        <v>10.6</v>
       </c>
       <c r="AA5">
-        <v>46.57451961</v>
+        <v>3.707999945</v>
       </c>
       <c r="AB5">
-        <v>10.6</v>
+        <v>41.976</v>
       </c>
       <c r="AC5">
-        <v>16.92218544</v>
+        <v>4.553658283</v>
       </c>
       <c r="AD5">
-        <v>3.707999945</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>41.976</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>4.553658283</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -1134,16 +1404,70 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:55">
       <c r="A6" s="1">
         <v>46</v>
       </c>
@@ -1151,16 +1475,16 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G6">
         <v>51.86239243</v>
@@ -1187,19 +1511,19 @@
         <v>38.22900009</v>
       </c>
       <c r="O6">
+        <v>2520</v>
+      </c>
+      <c r="P6">
         <v>25</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>36.77099991</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>72.98675034</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>20.36515297</v>
-      </c>
-      <c r="S6">
-        <v>2520</v>
       </c>
       <c r="T6">
         <v>14177437982</v>
@@ -1214,31 +1538,31 @@
         <v>7.11</v>
       </c>
       <c r="X6">
-        <v>2.55</v>
+        <v>56.5</v>
       </c>
       <c r="Y6">
-        <v>91.8724823</v>
+        <v>53.17355571</v>
       </c>
       <c r="Z6">
-        <v>56.5</v>
+        <v>7.4</v>
       </c>
       <c r="AA6">
-        <v>53.17355571</v>
+        <v>9.998000145000001</v>
       </c>
       <c r="AB6">
-        <v>7.4</v>
+        <v>64.95699999999999</v>
       </c>
       <c r="AC6">
-        <v>16.92218544</v>
+        <v>3.146204713</v>
       </c>
       <c r="AD6">
-        <v>9.998000145000001</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>64.95699999999999</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>3.146204713</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1247,16 +1571,70 @@
         <v>0</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:55">
       <c r="A7" s="1">
         <v>48</v>
       </c>
@@ -1264,16 +1642,16 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G7">
         <v>61.9</v>
@@ -1300,19 +1678,19 @@
         <v>50.375</v>
       </c>
       <c r="O7">
+        <v>1460</v>
+      </c>
+      <c r="P7">
         <v>5.986000061</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>43.63999939</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>36.6588334</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1.240430526</v>
-      </c>
-      <c r="S7">
-        <v>1460</v>
       </c>
       <c r="T7">
         <v>35372603446</v>
@@ -1327,31 +1705,31 @@
         <v>19.2742298</v>
       </c>
       <c r="X7">
-        <v>2.55</v>
+        <v>98.3</v>
       </c>
       <c r="Y7">
-        <v>43.90842056</v>
+        <v>26.27654966</v>
       </c>
       <c r="Z7">
-        <v>98.3</v>
+        <v>9.4</v>
       </c>
       <c r="AA7">
-        <v>26.27654966</v>
+        <v>2.747999907</v>
       </c>
       <c r="AB7">
-        <v>9.4</v>
+        <v>53.479</v>
       </c>
       <c r="AC7">
-        <v>13.97364016</v>
+        <v>3.881971936</v>
       </c>
       <c r="AD7">
-        <v>2.747999907</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <v>53.479</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <v>3.881971936</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -1360,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="AI7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
         <v>0</v>
@@ -1368,8 +1746,62 @@
       <c r="AK7">
         <v>0</v>
       </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>1</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:55">
       <c r="A8" s="1">
         <v>61</v>
       </c>
@@ -1377,16 +1809,16 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G8">
         <v>67.05870819</v>
@@ -1413,19 +1845,19 @@
         <v>54.96300125</v>
       </c>
       <c r="O8">
+        <v>13140</v>
+      </c>
+      <c r="P8">
         <v>8.237000464999999</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>36.79999924</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>65.9632886</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>0.772319187</v>
-      </c>
-      <c r="S8">
-        <v>13140</v>
       </c>
       <c r="T8">
         <v>21736500713</v>
@@ -1440,31 +1872,31 @@
         <v>18.86</v>
       </c>
       <c r="X8">
-        <v>2.55</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="Y8">
-        <v>91.8724823</v>
+        <v>46.69405811</v>
       </c>
       <c r="Z8">
-        <v>97.09999999999999</v>
+        <v>24</v>
       </c>
       <c r="AA8">
-        <v>46.69405811</v>
+        <v>5.494999886</v>
       </c>
       <c r="AB8">
-        <v>24</v>
+        <v>39.756</v>
       </c>
       <c r="AC8">
-        <v>8.298900808000001</v>
+        <v>4.514037661</v>
       </c>
       <c r="AD8">
-        <v>5.494999886</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>39.756</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>4.514037661</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -1473,16 +1905,70 @@
         <v>0</v>
       </c>
       <c r="AI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8">
         <v>0</v>
       </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
+        <v>1</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:55">
       <c r="A9" s="1">
         <v>75</v>
       </c>
@@ -1490,16 +1976,16 @@
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G9">
         <v>78.3</v>
@@ -1526,19 +2012,19 @@
         <v>44.72000122</v>
       </c>
       <c r="O9">
+        <v>1590</v>
+      </c>
+      <c r="P9">
         <v>14.10700035</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>41.17300034</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>39.52355867</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>8.604962551</v>
-      </c>
-      <c r="S9">
-        <v>1590</v>
       </c>
       <c r="T9">
         <v>39086625009</v>
@@ -1553,31 +2039,31 @@
         <v>25.51773743</v>
       </c>
       <c r="X9">
-        <v>2.55</v>
+        <v>63.4</v>
       </c>
       <c r="Y9">
-        <v>91.8724823</v>
+        <v>25.35736494</v>
       </c>
       <c r="Z9">
-        <v>63.4</v>
+        <v>10.9</v>
       </c>
       <c r="AA9">
-        <v>25.35736494</v>
+        <v>2.164000034</v>
       </c>
       <c r="AB9">
-        <v>10.9</v>
+        <v>53.392</v>
       </c>
       <c r="AC9">
-        <v>16.92218544</v>
+        <v>3.550496942</v>
       </c>
       <c r="AD9">
-        <v>2.164000034</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <v>53.392</v>
+        <v>0</v>
       </c>
       <c r="AF9">
-        <v>3.550496942</v>
+        <v>0</v>
       </c>
       <c r="AG9">
         <v>0</v>
@@ -1586,16 +2072,70 @@
         <v>0</v>
       </c>
       <c r="AI9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>1</v>
+      </c>
+      <c r="AV9">
+        <v>1</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:55">
       <c r="A10" s="1">
         <v>102</v>
       </c>
@@ -1603,16 +2143,16 @@
         <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G10">
         <v>36</v>
@@ -1639,19 +2179,19 @@
         <v>37.63899994</v>
       </c>
       <c r="O10">
+        <v>1260</v>
+      </c>
+      <c r="P10">
         <v>14.90200043</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>47.45899963</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>18.29698092</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1.335986481</v>
-      </c>
-      <c r="S10">
-        <v>1260</v>
       </c>
       <c r="T10">
         <v>61448046802</v>
@@ -1666,31 +2206,31 @@
         <v>16.5</v>
       </c>
       <c r="X10">
-        <v>5.9</v>
+        <v>53.5</v>
       </c>
       <c r="Y10">
-        <v>78.73303986000001</v>
+        <v>16.52198912</v>
       </c>
       <c r="Z10">
-        <v>53.5</v>
+        <v>19.1</v>
       </c>
       <c r="AA10">
-        <v>16.52198912</v>
+        <v>11.66699982</v>
       </c>
       <c r="AB10">
-        <v>19.1</v>
+        <v>25.197</v>
       </c>
       <c r="AC10">
-        <v>16.87697939</v>
+        <v>4.304922007</v>
       </c>
       <c r="AD10">
-        <v>11.66699982</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>25.197</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <v>4.304922007</v>
+        <v>0</v>
       </c>
       <c r="AG10">
         <v>0</v>
@@ -1707,8 +2247,62 @@
       <c r="AK10">
         <v>0</v>
       </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:55">
       <c r="A11" s="1">
         <v>146</v>
       </c>
@@ -1716,16 +2310,16 @@
         <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>56.37191391</v>
@@ -1752,19 +2346,19 @@
         <v>36.77999878</v>
       </c>
       <c r="O11">
+        <v>2980</v>
+      </c>
+      <c r="P11">
         <v>12.06200027</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>51.1590004</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>18.43512605</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>0.818201344</v>
-      </c>
-      <c r="S11">
-        <v>2980</v>
       </c>
       <c r="T11">
         <v>568499000000</v>
@@ -1779,31 +2373,31 @@
         <v>21</v>
       </c>
       <c r="X11">
-        <v>2.55</v>
+        <v>111.6</v>
       </c>
       <c r="Y11">
-        <v>91.8724823</v>
+        <v>41.60273017</v>
       </c>
       <c r="Z11">
-        <v>111.6</v>
+        <v>6.7</v>
       </c>
       <c r="AA11">
-        <v>41.60273017</v>
+        <v>4.559999943</v>
       </c>
       <c r="AB11">
-        <v>6.7</v>
+        <v>46.942</v>
       </c>
       <c r="AC11">
-        <v>16.92218544</v>
+        <v>4.48255153</v>
       </c>
       <c r="AD11">
-        <v>4.559999943</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <v>46.942</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>4.48255153</v>
+        <v>0</v>
       </c>
       <c r="AG11">
         <v>0</v>
@@ -1812,16 +2406,70 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>1</v>
+      </c>
+      <c r="AV11">
+        <v>1</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>1</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:55">
       <c r="A12" s="1">
         <v>163</v>
       </c>
@@ -1829,16 +2477,16 @@
         <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G12">
         <v>19.8</v>
@@ -1865,19 +2513,19 @@
         <v>68.45300293</v>
       </c>
       <c r="O12">
+        <v>700</v>
+      </c>
+      <c r="P12">
         <v>7.913000107</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>23.63400078</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>14.72211453</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>3.926137464</v>
-      </c>
-      <c r="S12">
-        <v>700</v>
       </c>
       <c r="T12">
         <v>8016591928</v>
@@ -1892,31 +2540,31 @@
         <v>10.6</v>
       </c>
       <c r="X12">
-        <v>2.55</v>
+        <v>43.4</v>
       </c>
       <c r="Y12">
-        <v>91.8724823</v>
+        <v>51.86310993</v>
       </c>
       <c r="Z12">
-        <v>43.4</v>
+        <v>63.8</v>
       </c>
       <c r="AA12">
-        <v>51.86310993</v>
+        <v>1.169999957</v>
       </c>
       <c r="AB12">
-        <v>63.8</v>
+        <v>27.841</v>
       </c>
       <c r="AC12">
-        <v>13.31802943</v>
+        <v>6.054470586</v>
       </c>
       <c r="AD12">
-        <v>1.169999957</v>
+        <v>0</v>
       </c>
       <c r="AE12">
-        <v>27.841</v>
+        <v>0</v>
       </c>
       <c r="AF12">
-        <v>6.054470586</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>0</v>
@@ -1925,16 +2573,70 @@
         <v>0</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK12">
         <v>0</v>
       </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>1</v>
+      </c>
+      <c r="AV12">
+        <v>1</v>
+      </c>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12">
+        <v>0</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:55">
       <c r="A13" s="1">
         <v>168</v>
       </c>
@@ -1942,16 +2644,16 @@
         <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G13">
         <v>61</v>
@@ -1978,19 +2680,19 @@
         <v>53.67399979</v>
       </c>
       <c r="O13">
+        <v>1030</v>
+      </c>
+      <c r="P13">
         <v>20.20499992</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>26.12100029</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>28.12071229</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>2.630373382</v>
-      </c>
-      <c r="S13">
-        <v>1030</v>
       </c>
       <c r="T13">
         <v>15304363138</v>
@@ -2005,31 +2707,31 @@
         <v>17.7</v>
       </c>
       <c r="X13">
-        <v>2.55</v>
+        <v>52.3</v>
       </c>
       <c r="Y13">
-        <v>91.8724823</v>
+        <v>35.99474681</v>
       </c>
       <c r="Z13">
-        <v>52.3</v>
+        <v>43.3</v>
       </c>
       <c r="AA13">
-        <v>35.99474681</v>
+        <v>6.356999874</v>
       </c>
       <c r="AB13">
-        <v>43.3</v>
+        <v>43.393</v>
       </c>
       <c r="AC13">
-        <v>19.6238999</v>
+        <v>3.697122779</v>
       </c>
       <c r="AD13">
-        <v>6.356999874</v>
+        <v>0</v>
       </c>
       <c r="AE13">
-        <v>43.393</v>
+        <v>0</v>
       </c>
       <c r="AF13">
-        <v>3.697122779</v>
+        <v>0</v>
       </c>
       <c r="AG13">
         <v>0</v>
@@ -2038,16 +2740,70 @@
         <v>0</v>
       </c>
       <c r="AI13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK13">
         <v>0</v>
       </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>1</v>
+      </c>
+      <c r="AV13">
+        <v>1</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
+        <v>0</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <v>0</v>
+      </c>
+      <c r="BC13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:55">
       <c r="A14" s="1">
         <v>186</v>
       </c>
@@ -2055,16 +2811,16 @@
         <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>44.9</v>
@@ -2091,19 +2847,19 @@
         <v>53.35599899</v>
       </c>
       <c r="O14">
+        <v>1830</v>
+      </c>
+      <c r="P14">
         <v>18.83399963</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>27.80999947</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>8.149134518</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1.523136574</v>
-      </c>
-      <c r="S14">
-        <v>1830</v>
       </c>
       <c r="T14">
         <v>82151588419</v>
@@ -2118,31 +2874,31 @@
         <v>24.64</v>
       </c>
       <c r="X14">
-        <v>2.55</v>
+        <v>69</v>
       </c>
       <c r="Y14">
-        <v>91.8724823</v>
+        <v>52.51987476</v>
       </c>
       <c r="Z14">
-        <v>69</v>
+        <v>24.3</v>
       </c>
       <c r="AA14">
-        <v>52.51987476</v>
+        <v>12.74800014</v>
       </c>
       <c r="AB14">
-        <v>24.3</v>
+        <v>33.623</v>
       </c>
       <c r="AC14">
-        <v>16.92218544</v>
+        <v>2.867143272</v>
       </c>
       <c r="AD14">
-        <v>12.74800014</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <v>33.623</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <v>2.867143272</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -2151,16 +2907,70 @@
         <v>0</v>
       </c>
       <c r="AI14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>1</v>
+      </c>
+      <c r="AV14">
+        <v>1</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <v>1</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:55">
       <c r="A15" s="1">
         <v>203</v>
       </c>
@@ -2168,16 +2978,16 @@
         <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G15">
         <v>20.4</v>
@@ -2204,19 +3014,19 @@
         <v>71.54699707</v>
       </c>
       <c r="O15">
+        <v>660</v>
+      </c>
+      <c r="P15">
         <v>6.887000084</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>21.56500053</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>18.17025675</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>3.878679401</v>
-      </c>
-      <c r="S15">
-        <v>660</v>
       </c>
       <c r="T15">
         <v>27291880327</v>
@@ -2231,31 +3041,31 @@
         <v>16.9</v>
       </c>
       <c r="X15">
-        <v>11.8</v>
+        <v>60.1</v>
       </c>
       <c r="Y15">
-        <v>91.8724823</v>
+        <v>61.38641667</v>
       </c>
       <c r="Z15">
-        <v>60.1</v>
+        <v>35</v>
       </c>
       <c r="AA15">
-        <v>61.38641667</v>
+        <v>1.907999992</v>
       </c>
       <c r="AB15">
-        <v>35</v>
+        <v>15.766</v>
       </c>
       <c r="AC15">
-        <v>16.92218544</v>
+        <v>5.459493493</v>
       </c>
       <c r="AD15">
-        <v>1.907999992</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>15.766</v>
+        <v>0</v>
       </c>
       <c r="AF15">
-        <v>5.459493493</v>
+        <v>0</v>
       </c>
       <c r="AG15">
         <v>0</v>
@@ -2267,10 +3077,64 @@
         <v>0</v>
       </c>
       <c r="AJ15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>0</v>
+      </c>
+      <c r="AV15">
+        <v>1</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>0</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>1</v>
+      </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BB15">
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include flagged of drop columns
</commit_message>
<xml_diff>
--- a/output/clean_data_central_africa.xlsx
+++ b/output/clean_data_central_africa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>country_index</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>m_urban_population_growth_pct</t>
+  </si>
+  <si>
+    <t>m_adult_literacy_pct</t>
+  </si>
+  <si>
+    <t>m_homicides_per_100k</t>
+  </si>
+  <si>
+    <t>m_tax_revenue_pct_gdp</t>
   </si>
   <si>
     <t>Central Africa 1</t>
@@ -617,13 +626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:BB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:54">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,8 +783,17 @@
       <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:54">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -783,16 +801,16 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -929,8 +947,17 @@
       <c r="AY2">
         <v>0</v>
       </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:54">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -938,16 +965,16 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G3">
         <v>72.91772460999999</v>
@@ -1084,8 +1111,17 @@
       <c r="AY3">
         <v>0</v>
       </c>
+      <c r="AZ3">
+        <v>1</v>
+      </c>
+      <c r="BA3">
+        <v>1</v>
+      </c>
+      <c r="BB3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:54">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1093,16 +1129,16 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G4">
         <v>51.86239243</v>
@@ -1239,8 +1275,17 @@
       <c r="AY4">
         <v>0</v>
       </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4">
+        <v>1</v>
+      </c>
+      <c r="BB4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:54">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1248,16 +1293,16 @@
         <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>19.8</v>
@@ -1394,8 +1439,17 @@
       <c r="AY5">
         <v>0</v>
       </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
+        <v>1</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:54">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1403,16 +1457,16 @@
         <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G6">
         <v>61</v>
@@ -1549,8 +1603,17 @@
       <c r="AY6">
         <v>0</v>
       </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:54">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1558,16 +1621,16 @@
         <v>203</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G7">
         <v>20.4</v>
@@ -1704,8 +1767,17 @@
       <c r="AY7">
         <v>0</v>
       </c>
+      <c r="AZ7">
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:54">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1713,16 +1785,16 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G8">
         <v>67.05870819</v>
@@ -1859,8 +1931,17 @@
       <c r="AY8">
         <v>0</v>
       </c>
+      <c r="AZ8">
+        <v>1</v>
+      </c>
+      <c r="BA8">
+        <v>1</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:54">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1868,16 +1949,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G9">
         <v>87.87672424</v>
@@ -2014,8 +2095,17 @@
       <c r="AY9">
         <v>0</v>
       </c>
+      <c r="AZ9">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:54">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2023,16 +2113,16 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G10">
         <v>13.5</v>
@@ -2169,8 +2259,17 @@
       <c r="AY10">
         <v>0</v>
       </c>
+      <c r="AZ10">
+        <v>1</v>
+      </c>
+      <c r="BA10">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:54">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2178,16 +2277,16 @@
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>61.9</v>
@@ -2324,8 +2423,17 @@
       <c r="AY11">
         <v>0</v>
       </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>1</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:54">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2333,16 +2441,16 @@
         <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G12">
         <v>78.3</v>
@@ -2479,8 +2587,17 @@
       <c r="AY12">
         <v>0</v>
       </c>
+      <c r="AZ12">
+        <v>1</v>
+      </c>
+      <c r="BA12">
+        <v>1</v>
+      </c>
+      <c r="BB12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:54">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2488,16 +2605,16 @@
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G13">
         <v>36</v>
@@ -2634,8 +2751,17 @@
       <c r="AY13">
         <v>0</v>
       </c>
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:54">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2643,16 +2769,16 @@
         <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>56.37191391</v>
@@ -2789,8 +2915,17 @@
       <c r="AY14">
         <v>0</v>
       </c>
+      <c r="AZ14">
+        <v>1</v>
+      </c>
+      <c r="BA14">
+        <v>1</v>
+      </c>
+      <c r="BB14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:54">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2798,16 +2933,16 @@
         <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G15">
         <v>44.9</v>
@@ -2943,6 +3078,15 @@
       </c>
       <c r="AY15">
         <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>1</v>
+      </c>
+      <c r="BA15">
+        <v>1</v>
+      </c>
+      <c r="BB15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>